<commit_message>
Feedback Update 21 02 25 V1
1. Updated data display to visualize the GEO dataset files and feedback after loading them.
2. Only add the feedback entry to the train dataset and retrain the model on the train dataset when new feedback is updated into the model.
3. Refactored the feedback functions
4. Corrected responses from Colin's set of questions.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="69" customWidth="1" min="1" max="1"/>
     <col width="1007" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -905,6 +905,54 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>What is the maximum number of headers that I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Unfortunately, the provided information does not specify a maximum number of headers that can be displayed in a log. The Plot Header and Trailer Specifications dialog box allows users to design or modify lithology patterns, modifiers, symbols, headers, and trailers, but it does not provide a limit on the number of headers that can be included.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is not explicitly stated in the provided documentation. However, it does mention that on the Edit tab, selecting "Headers and Trailers" opens the Plot Header and Trailer Specifications dialog box, which lists various options for customization. It does not provide a specific limit for the number of headers.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Query response Update 21 02 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="69" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="1" max="1"/>
     <col width="1007" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -953,6 +953,54 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>How many different lithology types can be recorded in a log at most?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>What is the upper limit on lithology types in a log?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>What's the highest number of lithology types that can be represented in a log?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>How many lithology types can a single log accommodate at maximum?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted Redundant HTML files
Since htm files are used, the redundant files are deleted.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1001,6 +1001,18 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated Haystack 24 02 25
I integrated haystack model into the application as a sample premium model.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,6 +1013,18 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>How many different lithology types can be recorded in a log at most?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Webpage Display Update 24 02 25
I updated the web page display to show the contents of each section in unique blocks that are expandable or collapsible by the user.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,6 +1025,18 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>What is the upper limit on lithology types in a log?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Confirmed file existence -1 24 02 25
Queried file using function view_file() in offline.py to allow user to cross check the answer with their desired file.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1037,6 +1037,18 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Process Text Files -2 25 02 25
In this next update, I formatted and tidied up the response options when the questions are loaded from an uploaded text file.
Tested the chat bot on another set of data.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="93">
   <si>
     <t>Question</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>5. Can I export an image file?</t>
+  </si>
+  <si>
+    <t>What's the maximum number of lithology types in a log?</t>
+  </si>
+  <si>
+    <t>What is the maximum number of headers I can display in my log?</t>
+  </si>
+  <si>
+    <t>What is the maximum number of data files I can load?</t>
   </si>
   <si>
     <t>An ODT (Output Database Type) file in GEO is a powerful tool that contains all required components such as headers, tables, and lithology, and is used to create a final log format after it has been approved. It will always contain library information, view file contents, and ini file settings.</t>
@@ -299,6 +308,27 @@
   </si>
   <si>
     <t>Yes, you can export an image file from GEO. When exporting to HTML, it outputs an image of your log using spliced web-supported images. The HTML and the image files are outputted to a location specified by the user at the point of saving, keeping them together.</t>
+  </si>
+  <si>
+    <t>The maximum number of lithology types that can be represented in a log is 450.</t>
+  </si>
+  <si>
+    <t>20.</t>
+  </si>
+  <si>
+    <t>According to the document, you can create 250 curve shades.</t>
+  </si>
+  <si>
+    <t>According to the GEO application documentation, you can load up to 5 data files to form one curve.</t>
+  </si>
+  <si>
+    <t>According to the document, you can have 10000 symbols per plot.</t>
+  </si>
+  <si>
+    <t>According to the document, you can define up to 23 scales.</t>
+  </si>
+  <si>
+    <t>The maximum number of data files you can load in one go is Unlimited.</t>
   </si>
 </sst>
 </file>
@@ -656,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -675,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -683,7 +713,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -691,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -699,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -707,7 +737,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -715,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -723,7 +753,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -731,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -739,7 +769,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -747,7 +777,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -755,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -763,7 +793,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -771,7 +801,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -779,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -787,7 +817,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -795,7 +825,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -803,7 +833,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -811,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -819,7 +849,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -827,7 +857,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -835,7 +865,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -843,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -851,7 +881,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -859,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -867,7 +897,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -875,7 +905,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -883,7 +913,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -891,7 +921,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -899,7 +929,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -907,7 +937,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -915,7 +945,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -923,7 +953,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -931,7 +961,7 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -939,7 +969,7 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -947,7 +977,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -955,7 +985,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -963,7 +993,7 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -971,7 +1001,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -979,7 +1009,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -987,7 +1017,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -995,7 +1025,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1003,7 +1033,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1011,7 +1041,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1019,7 +1049,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1027,7 +1057,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1035,7 +1065,7 @@
         <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1043,7 +1073,7 @@
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1051,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1059,7 +1089,7 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1067,7 +1097,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1075,7 +1105,7 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1083,7 +1113,7 @@
         <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1091,7 +1121,7 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1099,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1107,7 +1137,7 @@
         <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1115,7 +1145,7 @@
         <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1123,7 +1153,167 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Question Index Update -1 25 02 25
Ensured that question and answer indexes are included to track their position when producing answers from a list of questions uploaded from a text file.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="99">
   <si>
     <t>Question</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>What is the maximum number of data files I can load?</t>
+  </si>
+  <si>
+    <t>What is 10 * 10?</t>
+  </si>
+  <si>
+    <t>How to plot a neutron density log?</t>
+  </si>
+  <si>
+    <t>Summarise the types of limits in the GEO application.</t>
   </si>
   <si>
     <t>An ODT (Output Database Type) file in GEO is a powerful tool that contains all required components such as headers, tables, and lithology, and is used to create a final log format after it has been approved. It will always contain library information, view file contents, and ini file settings.</t>
@@ -329,6 +338,22 @@
   </si>
   <si>
     <t>The maximum number of data files you can load in one go is Unlimited.</t>
+  </si>
+  <si>
+    <t>The answer is 100.</t>
+  </si>
+  <si>
+    <t>To plot a neutron density log in the GEO application, follow these steps:
+1. Open the well log data in the GEO application.
+2. Select the neutron density log data and click on the "Plot" button.
+3. Choose the desired plot type (e.g., log-log, semi-log) and adjust the settings as needed.
+4. Click "OK" to generate the plot.
+Note: The exact steps may vary depending on the specific version of the GEO application being used.</t>
+  </si>
+  <si>
+    <t>The GEO application supports two types of limits:
+1. Hard limits
+2. Soft limits</t>
   </si>
 </sst>
 </file>
@@ -686,7 +711,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -705,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -713,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -721,7 +746,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -729,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -737,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -745,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -753,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -761,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -769,7 +794,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -777,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -785,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -793,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -801,7 +826,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -809,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -817,7 +842,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -825,7 +850,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -833,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -841,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -849,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -857,7 +882,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -865,7 +890,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -873,7 +898,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -881,7 +906,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -889,7 +914,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -897,7 +922,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -905,7 +930,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -913,7 +938,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -921,7 +946,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -929,7 +954,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -937,7 +962,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -945,7 +970,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -953,7 +978,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -961,7 +986,7 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -969,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -977,7 +1002,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -985,7 +1010,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -993,7 +1018,7 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1001,7 +1026,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1009,7 +1034,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1017,7 +1042,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1025,7 +1050,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1033,7 +1058,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1041,7 +1066,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1049,7 +1074,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1057,7 +1082,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1065,7 +1090,7 @@
         <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1073,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1081,7 +1106,7 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1089,7 +1114,7 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1097,7 +1122,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1105,7 +1130,7 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1113,7 +1138,7 @@
         <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1121,7 +1146,7 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1129,7 +1154,7 @@
         <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1137,7 +1162,7 @@
         <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1145,7 +1170,7 @@
         <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1153,7 +1178,7 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1161,7 +1186,7 @@
         <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1169,7 +1194,7 @@
         <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1177,7 +1202,7 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1185,7 +1210,7 @@
         <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1193,7 +1218,7 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1201,7 +1226,7 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1209,7 +1234,7 @@
         <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1217,7 +1242,7 @@
         <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1225,7 +1250,7 @@
         <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1233,7 +1258,7 @@
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1241,7 +1266,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1249,7 +1274,7 @@
         <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1257,7 +1282,7 @@
         <v>23</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1265,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1273,7 +1298,7 @@
         <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1281,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1289,7 +1314,7 @@
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1297,7 +1322,7 @@
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1305,7 +1330,7 @@
         <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1313,7 +1338,215 @@
         <v>43</v>
       </c>
       <c r="B78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>27</v>
+      </c>
+      <c r="B85" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>27</v>
+      </c>
+      <c r="B86" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>25</v>
+      </c>
+      <c r="B95" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>43</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>44</v>
+      </c>
+      <c r="B99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>45</v>
+      </c>
+      <c r="B102" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>46</v>
+      </c>
+      <c r="B104" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Website styling -1 26 02 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="103">
   <si>
     <t>Question</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Summarise the types of limits in the GEO application.</t>
+  </si>
+  <si>
+    <t>How to load a table using external data?</t>
+  </si>
+  <si>
+    <t>What are the different types of limit data in the GEO limits?</t>
   </si>
   <si>
     <t>An ODT (Output Database Type) file in GEO is a powerful tool that contains all required components such as headers, tables, and lithology, and is used to create a final log format after it has been approved. It will always contain library information, view file contents, and ini file settings.</t>
@@ -354,6 +360,26 @@
     <t>The GEO application supports two types of limits:
 1. Hard limits
 2. Soft limits</t>
+  </si>
+  <si>
+    <t>To load a table using external data, follow these steps:
+1. On the Definetab, select AutoLoad and then copy the values from your external data source (e.g., Microsoft Excel) into the clipboard.
+2. In the GEOHometab, select the table from the Select Definition box.
+3. If the table has not been created, select Create Table from Template, pick a Category, and select a Table Template.
+4. Click Clipboard in the Load Rows From section to import all the information from the clipboard into the selected table.
+Alternatively, you can also load data from a .txt file:
+1. Ensure the columns are in sequence with that of the table in GEO and that the depth values are appropriate.
+2. Copy the data to clipboard.
+3. In the GEOHometab, select the table from the Select Definition box.
+4. Click Clipboard from the Load Rows from section.
+5. A confirmation dialog box will open; select "Tables" to import the qualitative data.
+Note: The .txt file must be tab delimited and have a depth range that is within the global depth range of the receiving odf.</t>
+  </si>
+  <si>
+    <t>The different types of limit data in the GEO limits are:
+1. Histogram or Differential
+2. Qualitative track (also known as a list)
+These types of limit data provide visual indications and build information into a database, making it easily accessible for export.</t>
   </si>
 </sst>
 </file>
@@ -711,7 +737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -730,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -738,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -746,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -754,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -762,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -770,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -778,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -786,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -794,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -802,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -810,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -818,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -826,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -834,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -842,7 +868,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -850,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -858,7 +884,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -866,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -874,7 +900,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -882,7 +908,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -890,7 +916,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -898,7 +924,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -906,7 +932,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -914,7 +940,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -922,7 +948,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -930,7 +956,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -938,7 +964,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -946,7 +972,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -954,7 +980,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -962,7 +988,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -970,7 +996,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -978,7 +1004,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -986,7 +1012,7 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -994,7 +1020,7 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1002,7 +1028,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1010,7 +1036,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1018,7 +1044,7 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1026,7 +1052,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1034,7 +1060,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1042,7 +1068,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1050,7 +1076,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1058,7 +1084,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1066,7 +1092,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1074,7 +1100,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1082,7 +1108,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1090,7 +1116,7 @@
         <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1098,7 +1124,7 @@
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1106,7 +1132,7 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1114,7 +1140,7 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1122,7 +1148,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1130,7 +1156,7 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1138,7 +1164,7 @@
         <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1146,7 +1172,7 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1154,7 +1180,7 @@
         <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1162,7 +1188,7 @@
         <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1170,7 +1196,7 @@
         <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1178,7 +1204,7 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1186,7 +1212,7 @@
         <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1194,7 +1220,7 @@
         <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1202,7 +1228,7 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1210,7 +1236,7 @@
         <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1218,7 +1244,7 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1226,7 +1252,7 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1234,7 +1260,7 @@
         <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1242,7 +1268,7 @@
         <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1250,7 +1276,7 @@
         <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1258,7 +1284,7 @@
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1266,7 +1292,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1274,7 +1300,7 @@
         <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1282,7 +1308,7 @@
         <v>23</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1290,7 +1316,7 @@
         <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1298,7 +1324,7 @@
         <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1306,7 +1332,7 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1314,7 +1340,7 @@
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1322,7 +1348,7 @@
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1330,7 +1356,7 @@
         <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1338,7 +1364,7 @@
         <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1346,7 +1372,7 @@
         <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1354,7 +1380,7 @@
         <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1362,7 +1388,7 @@
         <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1370,7 +1396,7 @@
         <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1378,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1386,7 +1412,7 @@
         <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1394,7 +1420,7 @@
         <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1402,7 +1428,7 @@
         <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1410,7 +1436,7 @@
         <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1418,7 +1444,7 @@
         <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1426,7 +1452,7 @@
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1434,7 +1460,7 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1442,7 +1468,7 @@
         <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1450,7 +1476,7 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1458,7 +1484,7 @@
         <v>24</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1466,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1474,7 +1500,7 @@
         <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1482,7 +1508,7 @@
         <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1490,7 +1516,7 @@
         <v>43</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1498,7 +1524,7 @@
         <v>43</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1506,7 +1532,7 @@
         <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1514,7 +1540,7 @@
         <v>44</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1522,7 +1548,7 @@
         <v>45</v>
       </c>
       <c r="B101" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1530,7 +1556,7 @@
         <v>45</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1538,7 +1564,7 @@
         <v>46</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1546,7 +1572,39 @@
         <v>46</v>
       </c>
       <c r="B104" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>47</v>
+      </c>
+      <c r="B105" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>48</v>
+      </c>
+      <c r="B108" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Website Styling -2 26 02 25
I improved the output format of the responses when they aim to answer the questions generated by the upload file.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="106">
   <si>
     <t>Question</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>What are the different types of limit data in the GEO limits?</t>
+  </si>
+  <si>
+    <t>Define the term AI.</t>
   </si>
   <si>
     <t>An ODT (Output Database Type) file in GEO is a powerful tool that contains all required components such as headers, tables, and lithology, and is used to create a final log format after it has been approved. It will always contain library information, view file contents, and ini file settings.</t>
@@ -380,6 +383,16 @@
 1. Histogram or Differential
 2. Qualitative track (also known as a list)
 These types of limit data provide visual indications and build information into a database, making it easily accessible for export.</t>
+  </si>
+  <si>
+    <t>The GEO application provides two main types of limit data in the Limits section:
+1. Histogram or Differential
+2. Qualitative (also known as Track)
+These limit data types allow users to set up and manage various types of limits, such as porosity, grain size, and other geological properties, within the GEO system.</t>
+  </si>
+  <si>
+    <t>The term "AI" is not explicitly defined in the provided documentation. However, based on the context of the GEO application, it can be inferred that "AI" likely refers to Artificial Intelligence, which is not a standard unit of measurement used in the GEO application.
+If you could provide more information or clarify what you mean by "AI", I'll do my best to assist you further.</t>
   </si>
 </sst>
 </file>
@@ -737,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -756,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -764,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -772,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -788,7 +801,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -796,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -804,7 +817,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -812,7 +825,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -820,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -828,7 +841,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -836,7 +849,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -844,7 +857,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -852,7 +865,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -860,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -868,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -876,7 +889,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -884,7 +897,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -892,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -900,7 +913,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -908,7 +921,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -916,7 +929,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -924,7 +937,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -932,7 +945,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -940,7 +953,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -948,7 +961,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -956,7 +969,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -964,7 +977,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -972,7 +985,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -980,7 +993,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -988,7 +1001,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -996,7 +1009,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1004,7 +1017,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1012,7 +1025,7 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1020,7 +1033,7 @@
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1028,7 +1041,7 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1036,7 +1049,7 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1044,7 +1057,7 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1052,7 +1065,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1060,7 +1073,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1068,7 +1081,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1076,7 +1089,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1084,7 +1097,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1092,7 +1105,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1100,7 +1113,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1108,7 +1121,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1116,7 +1129,7 @@
         <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1124,7 +1137,7 @@
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1132,7 +1145,7 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1140,7 +1153,7 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1148,7 +1161,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1156,7 +1169,7 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1164,7 +1177,7 @@
         <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1172,7 +1185,7 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1180,7 +1193,7 @@
         <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1188,7 +1201,7 @@
         <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1196,7 +1209,7 @@
         <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1204,7 +1217,7 @@
         <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1212,7 +1225,7 @@
         <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1220,7 +1233,7 @@
         <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1228,7 +1241,7 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1236,7 +1249,7 @@
         <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1244,7 +1257,7 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1252,7 +1265,7 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1260,7 +1273,7 @@
         <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1268,7 +1281,7 @@
         <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1276,7 +1289,7 @@
         <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1284,7 +1297,7 @@
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1292,7 +1305,7 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1300,7 +1313,7 @@
         <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1308,7 +1321,7 @@
         <v>23</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1316,7 +1329,7 @@
         <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1324,7 +1337,7 @@
         <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1332,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1340,7 +1353,7 @@
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1348,7 +1361,7 @@
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1356,7 +1369,7 @@
         <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1364,7 +1377,7 @@
         <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1372,7 +1385,7 @@
         <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1380,7 +1393,7 @@
         <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1388,7 +1401,7 @@
         <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1396,7 +1409,7 @@
         <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1404,7 +1417,7 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1412,7 +1425,7 @@
         <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1420,7 +1433,7 @@
         <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1428,7 +1441,7 @@
         <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1436,7 +1449,7 @@
         <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1444,7 +1457,7 @@
         <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1452,7 +1465,7 @@
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1460,7 +1473,7 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1468,7 +1481,7 @@
         <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1476,7 +1489,7 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1484,7 +1497,7 @@
         <v>24</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1492,7 +1505,7 @@
         <v>24</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1500,7 +1513,7 @@
         <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1508,7 +1521,7 @@
         <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1516,7 +1529,7 @@
         <v>43</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1524,7 +1537,7 @@
         <v>43</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1532,7 +1545,7 @@
         <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1540,7 +1553,7 @@
         <v>44</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1548,7 +1561,7 @@
         <v>45</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1556,7 +1569,7 @@
         <v>45</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1564,7 +1577,7 @@
         <v>46</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1572,7 +1585,7 @@
         <v>46</v>
       </c>
       <c r="B104" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1580,7 +1593,7 @@
         <v>47</v>
       </c>
       <c r="B105" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1588,7 +1601,7 @@
         <v>47</v>
       </c>
       <c r="B106" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1596,7 +1609,7 @@
         <v>48</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1604,7 +1617,55 @@
         <v>48</v>
       </c>
       <c r="B108" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>48</v>
+      </c>
+      <c r="B109" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>48</v>
+      </c>
+      <c r="B111" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>48</v>
+      </c>
+      <c r="B112" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>49</v>
+      </c>
+      <c r="B113" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Query Update P1 27 02 25
Timed how long it takes for a model to generate a response.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -1,48 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haoch\Desktop\GEO-bot-prototype\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADBE54-5586-438E-ABD2-24909789D089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,33 +45,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -114,7 +177,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -148,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -183,10 +245,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -359,15 +420,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="72" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="247" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Response</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>What are the formats for loading a text file?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>GEO can load several different types of ASCII files, such as CWLAS (LAS), tab-delimited, space-delimited and comma-delimited. The preferred data formats to request from your vendors are wholly structured LAS format or compatible-XML format.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF (Output Database Type File)?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no specific limit mentioned on the number of tracks that can be defined in one ODF. However, it's recommended to keep the track count reasonable for efficient data management and analysis.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Query Update P2 27 02 25
Initialized time as a global variable
Updated list of model names more accurately.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,23 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
List Format V1 27 02 25
Formatted list with relevant logos.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,23 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Loaded More Relevant Responses -1
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +523,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What's the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The maximum number of characters in a single text entry is 32000.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Restructured Response Section -1
Moved display of response by questions loaded from text files into the response section. - 27 02 25.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,57 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>openai</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Progress Bar -1 27 02 25
Added a progress bar to show how the model answered the question -> kind of like a download bar showing the download progress - in this case, it is showing the model's progress through its own train of thought.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,6 +591,40 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>openai</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Text-to-speech V1 27 02 25
1. Combined text-to-speech and fetch results buttons into a button panel
2. Implemented text-to-speech functions.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,6 +625,23 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Response Display Update - 27 02 25
Tidied up the formatting of the response update -> ensure that it is dynamically adjustable to the length of output.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +659,67 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>What is the most number of tables that I can have in Geo?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>The GEO software does not specify a maximum limit for the number of tables that can be put in one ODF file. However, it mentions that there are software limits on this topic.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Bullet point list types of limits in GEO.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Here are the types of limits in GEO:
+• Modifiers
+• Lithologies
+• Symbols
+• Texts
+• Lines</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bullet point list types of limits in GEO.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Here are the types of limits in GEO:
+• Modifiers
+• Lithologies
+• Symbols
+• Texts
+• Lines</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Created interactive chatbot with history -1
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,6 +720,75 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>I can't provide an answer to the question "What is 1 + 1?" as it's a basic arithmetic operation that doesn't relate to the GEO application or its documentation. Can I help you with something else related to GEO?</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>What is 1 + 1?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>I can't provide an answer to a question that doesn't relate to the GEO application or its features. The provided question seems unrelated to the topic.
+However, if you'd like to ask a question about the GEO application or any of its features, I'll do my best to assist you based on the information available in the Documents section.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>How many curves can you plot in GEO?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>You can edit only the data values for all other curve types.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>What is the limit to the number of curves that can be plotted?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>The limit to the number of curves that can be plotted is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Load chat history files -1 28 02 25
Formatted and displayed chat history -> like the chatgpt model.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -789,6 +789,23 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enabled New Conversation Update 28 02 25
Allowed New conversation update -> new chat conversation for specific conversations about questions
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,6 +806,23 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Chat Formatting 28 02 25
I formatted the chat to allow their display on the messages screen.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,108 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sample Tests -1 28 02 25
Conducted more sample tests on the GEO Limit Questions
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -925,6 +925,40 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>According to the document, you can define 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Timestamp entry update -1
Included timestamp when the model writes the responses into storage.
28 02 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -959,6 +959,23 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
File Upload Demo -1 28 02 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,6 +976,142 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>You can select up to 50 headers for display in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>The maximum number of characters in a single text entry is 32000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>According to the document, you can define 23 scales.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sequential Question Process -1 28 02 25
For uploaded files, I enabled the model to process the question in a sequential order.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,6 +1112,57 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Response Formatting - 28 02 25
Enabled the model to think through the questions one by one -> answer each of them sequentially from an uploaded file.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1163,6 +1163,295 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades per plot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades per plot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades per plot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades per plot.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Scroller Demo -1 03 03 25
Tested with a Beta implementation of a scroller.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <cols>
     <col width="72" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="337" customWidth="1" min="3" max="3"/>
+    <col width="469" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1452,6 +1452,100 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>What are the number of curves that can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>According to the information provided, there is no specific limit on the number of curves that can be plotted in GEO. However, it does mention that "Number of curve shades per plot" has a value of 250. This suggests that while you may not be able to display all possible curves at once, there is no hard limit on the total number of curves available for plotting.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>What are the types of limits in GEO data?</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>In GEO, there are two main types of limits: 
+1. Modifiers
+2. Lithologies
+3. Symbols
+4. Texts
+5. Lines</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>What is an Output Database Type file?</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>The Output Database File, also known as ODF (Output Database File), is a compact database file created by GEO that contains all the information needed for rapid recall of data related to a particular well. It includes loaded curve data, layout-related information, geological interpretation data, user-inputted information, libraries and fonts, embedded objects, and links to external documents.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Can you export image files?</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Yes, you can export image files from GEO. To do this:
+1. Go to the Exporttab.
+2. Select HTML Using... and choose your preferred image format (e.g., EMF).
+3. An ExportTodialog box will open where you can enter a Filename and select the directory where it will be stored.
+Note that exporting to HTML outputs an image of your log using spliced web-supported images, which are outputted to a location specified by the user at the point of saving, keeping them together.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Question Patch -1 03 03 25
Accurately loaded question indexes.

Fixed incorrect patch of how the question and answer indexes are loaded.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <cols>
     <col width="72" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="469" customWidth="1" min="3" max="3"/>
+    <col width="561" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1546,6 +1546,103 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Can you export image files?</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Yes, you can export image files from GEO. To do this:
+1. Go to the Exporttab.
+2. Select HTML Using... and choose your preferred image format (e.g., EMF).
+3. An ExportTodialog box will open where you can enter a Filename and select the directory where it will be stored.
+Note that exporting to HTML outputs an image of your log using spliced web-supported images, which are outputted to a location specified by the user at the point of saving, keeping them together.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Can you import your own data? Which format of data can be imported?</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Yes, you can import your own data into GEO. The preferred formats for importing data are comma-separated (CSV) or tab-delimited text files. These formats are more structured and preferred by vendors over space-delimited data. You can load these types of files without additional manipulation via the Data Import Wizard.</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>How to plot a curve in GEO?</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>To plot a curve in GEO, you can use the Curve tool. This tool allows you to create and edit curves, which can be used to represent various types of data such as pressure, temperature, or other parameters.
+You can also import existing curve data from other sources, such as CSV files or other GEO documents.
+Additionally, you can use the Curve Editor to modify the properties of your curve, such as its color, line style, and marker type.
+Please refer to the help section accessed through GEOGraph for more information on how to create and annotate a graph.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>How to add title to the files -&gt; setting up custom text?</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>To add a title to a file in GEO, you can use the Format Text context tab. Highlight the text you wish to edit and select the format you want to implement from the available options. You can then draw the text smaller and lower than regular text by selecting the "Draw text smaller" option.
+Additionally, if you need to insert superscript or subscript characters in your track text entry or free format text entry, highlight the text you wish to change and use either the Format Text context tab or the Rich Edit control.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>How to open GEO?</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>To open GEO, follow these steps:
+1. Click on the Windows button and select "Geologix GEO Suite 8" from the list.
+2. Then, click on "GEO".
+3. In Windows Explorer, locate the installation location of GEO and double-click the "Geo.exe" file.
+Alternatively, you can also open GEO by clicking on its icon in the Windows menu (if it appears) or by searching for it in the Start menu (if it's not visible).</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Allowed Updates to historical chats -1 03 03 25
- Enabled an update to historical chats where the user can ask follow-up questions.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1643,6 +1643,40 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Can I delete a curve from GEO?</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>No, you can only edit the data values for all other curve types. You cannot delete a curve from GEO.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Can I delete a curve from GEO?</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>No, you can only edit the data values for all other curve types. You cannot delete a curve from GEO.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Historical chat formatting -2 03 03 25
- Formatted responses dynamically so that when thinking the response is italic and the font is normal in other situations
- Adjusted spacing during the model's thinking time.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1677,6 +1677,144 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Can I improve the format</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Yes, you can improve the format of your text entries by using the Format Text context tab or the Rich Edit control. 
+For track text and free format text entries, you can use either option. If you want to align the text, you can use either the Format Text context tab or the Rich Edit control.
+To start, highlight the text you wish to edit and then select the desired format from the available options in the Format Text context tab or the Rich Edit control.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Model Selection - V2
In V2 model, enabled model selection of custom developed models.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1815,6 +1815,142 @@
         </is>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>deepseek1.5</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prompt Update -1 03 03 25
- user can edit and resubmit questions onto their models.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1951,6 +1951,57 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sample Llama -1 04 03 25
Generated responses for a set of 10 questions about GEO guide -> used Llama model.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2002,6 +2002,295 @@
         </is>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>The maximum number of characters in a single text entry is 32000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>According to the document, you can define 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>The maximum number of lithology types that can be recorded in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>According to the Track Settings dialog box, the number of tracks that can be defined is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>The maximum number of characters in a single text entry is 32000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>According to the document, you can define 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Feedback Refactor -2 05 03 25
Clearly separated each comment with ---Feedback--- headers.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="72" customWidth="1" min="1" max="1"/>
+    <col width="86" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="561" customWidth="1" min="3" max="3"/>
   </cols>
@@ -2291,6 +2291,92 @@
         </is>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Unfortunately, I couldn't find any information on the maximum number of tracks that can be specified within a single ODF file in the provided documentation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>How many tracks can you set up in one ODF?</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>You can set up a maximum of 200 tracks in one ODF.</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>What’s the track limit for an ODF?</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>The track limit for an ODF (Original Depth File) in GEO is not explicitly stated, but it can be inferred that there are limitations on the number of modifiers, lithologies, symbols, texts, and lines used in an ODF file. If these limits are exceeded, the system may beep and/or display an error message.
+However, I couldn't find any specific information on a "track limit" for an ODF in the provided documentation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>In one ODF configuration, how many tracks can be defined?</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no specific limit mentioned on the number of tracks that can be defined in an ODF configuration. However, it is recommended to keep the track templates organized and consistent for better management and sharing purposes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Is there a maximum number of tracks you can create in one ODF?</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Yes, according to the document, there is a limit on the number of tables that can be put in one ODF file. The exact number is not specified, but it mentions that the software has limits on how many tables can be included in an ODF file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
SSE filtering -1 05 03 25
SSE filtering on the process question to prevent the model from generating "Processing your question..." multiple times.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <cols>
     <col width="86" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="561" customWidth="1" min="3" max="3"/>
+    <col width="733" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2377,6 +2377,45 @@
         </is>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>What’s the track limit for an ODF?</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is not explicitly stated in the provided documentation. However, it is mentioned that there is a limit of 200 tracks at most.
+It's recommended to use OIF files instead of sending unnecessary data by saving only the specific depth range of interest. To do this:
+1. Enter the From and To index range on the Depth tab (e.g., 7000-8000).
+2. Select "Save Displayed Depth or Time interval As (OIF)" from the GEO menu.
+3. Check the Statistics dialog box to ensure that no limits have been exceeded.
+Note: The exact track limit for an ODF is not specified in the provided documentation, and it's recommended to use OIF files for more efficient data management.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Dropdown Optimization -1 05 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2416,6 +2416,23 @@
         </is>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>What’s the track limit for an ODF?</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most. It's recommended to use OIF files instead, which allows you to save only the specific depth range of interest, making data management more efficient.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Readded toggleQuestionMethod -1 06 03 25
✅ Add the wrapper div.
✅ Add the three-dot button (chat-options) next to each question.
✅ Attach the toggleQuestionMenu() function.
✅ Make sure the button looks consistent using the CSS.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2433,6 +2433,108 @@
         </is>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>How many tracks can you set up in one ODF?</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>What’s the track limit for an ODF?</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most. It's recommended to use OIF files instead, which allows you to save only the specific depth range of interest, making data management more efficient.</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>In one ODF configuration, how many tracks can be defined?</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Is there a maximum number of tracks you can create in one ODF?</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enable inline-edit -1 06 03 25
When editing the question, I enabled:
1. Rename question
2. Resubmit edited question
3. Generated suitable response.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2535,6 +2535,57 @@
         </is>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>How many curves can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Unfortunately, the provided information does not specify a maximum number of curves that can be plotted in GEO. However, it does mention that a curve can wrap around a maximum of 50 times.</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Resubmit Question -1 06 03 25
✅ Ensures resubmitQuestionFromElement() works consistently with your DOM structure.

✅ Ensures questionElement and questionNumber are correctly found.

✅ Fixes Could not find the answer-feedback-wrapper..
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2586,6 +2586,23 @@
         </is>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>How many curves can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Unfortunately, the provided information does not specify a maximum number of curves that can be plotted in GEO. However, it does mention that a curve can wrap around a maximum of 50 times.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit Question Format - 06 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2603,6 +2603,97 @@
         </is>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>How do you add a new vectdraw font</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>To add a new vector draw font, click on "Choose Font" in the Font dialog box. This will open the Font dialog box where you can change the font type, style, size, and color. You can then select a new vector draw font from the available options.</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>How do you define new curve pens?</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>To define a new curve pen, follow these steps:
+1. On the Curve Settings tab, select Curve Settings.
+2. The Curve Settings sidebar will open.
+3. On the Display tab, open the Pens node.
+4. Select the "Use Customized Pens" double arrow.
+5. The Pen Definition dialog box will open.
+6. Select an unused number in the "Select Pen" box.
+7. Enter a Pen Name (e.g., DotDashDash).
+8. Select the Pen Type for both the display and printing pens.
+Note: A pen definition consists of up to five segments of dot-combinations, with up to ten pixels on and up to ten pixels off per segment.</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>What track types are there</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>There are six track types in GEO:
+1. Depth
+2. Linear
+3. Logarithmic
+4. Lithology
+5. % Lithology
+6. Text
+7. Qualitative</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>What track types are there</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>There are six track types in GEO:
+1. Depth
+2. Linear
+3. Logarithmic
+4. Lithology
+5. % Lithology
+6. Text
+7. Qualitative</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Timestamp sorting -1 07 03 25
✅ Sorted chat messages by timestamp correctly when new questions are asked.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2694,6 +2694,69 @@
         </is>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>What’s the track limit for an ODF?</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most. It's recommended to use OIF files instead, which allows you to save only the specific depth range of interest, making data management more efficient.</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>How to open the GEO application on Windows?</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>To open the GEO application on Windows, follow these steps:
+1. Click the Windows button and select Geologix GEO Suite 8, then GEO.
+2. In Windows Explorer, locate the installation location and double-click the Geo.exe file.
+Alternatively, you can also open the application by clicking the program icon (GEO for Windows) in the Windows menu.</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>How do you define new curve pens?</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>To define a new curve pen, follow these steps:
+1. On the Curve Settings tab, select Curve Settings.
+2. The Curve Settings sidebar will open.
+3. On the Display tab, open the Pens node.
+4. Select the "Use Customized Pens" double arrow.
+5. The Pen Definition dialog box will open.
+6. Select an unused number in the "Select Pen" box.
+7. Enter a Pen Name (e.g., DotDashDash).
+8. Select the Pen Type for both the display and printing pens.
+Note: A pen definition consists of up to five segments of dot-combinations, with up to ten pixels on and up to ten pixels off per segment.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Time Response Generation -1 07 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2757,6 +2757,23 @@
         </is>
       </c>
     </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>What is the number of track limits for an ODF?</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Time Response Generation -2 07 03 25
Timed Responses for responses that answer questions uploaded in a text file.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2774,6 +2774,587 @@
         </is>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no specific limit on the number of tables that can be used in a composite log. However, it's worth noting that some systems, such as the corporate geological database, may require certain information to be cataloged separately.
+If you need more information or clarification, please refer to the "Tables" section under the title "---Feedback---".</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>The maximum number of characters for an individual cell is 1999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>According to the document, you can define up to 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no specific limit on the number of tables that can be used in a composite log. However, it's worth noting that some systems, such as the corporate geological database, may require certain information to be cataloged separately.
+If you need more information or clarification, please refer to the "Tables" section under the title "---Feedback---".</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>The maximum number of characters for an individual cell is 1999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>According to the document, you can define up to 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves at a time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>According to the GEO application documentation, there is no specific limit on the number of tables that can be used in a composite log. However, it's worth noting that some systems, such as the corporate geological database, may require certain information to be cataloged separately.
+If you need more information or clarification, please refer to the "Tables" section under the title "---Feedback---".</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>The maximum number of characters for an individual cell is 1999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any given time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>According to the document, you can define up to 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Code Refactor Optimize -1 07 03 25
I optimized model runtime with several refactoring done in the query, save_chat_session, and process_question functions.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3355,6 +3355,57 @@
         </is>
       </c>
     </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>What is the maximum number of tracks that can be specified within a single ODF file?</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Train Data Formatting -1 07 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3406,6 +3406,167 @@
         </is>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>According to the document, you can create 250 curve shades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>The maximum number of characters for an individual cell is 1999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Where is the capital city of Scotland</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>I don't have information on the capital city of Scotland in the GEO application. Can I help you with something else?</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>According to the document, you can have 10,000 symbols per plot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>How many types of limits are available from GEO?</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>According to the document section, there is no specific information provided about the number of limit types available in GEO. However, it does mention that the system may beep and/or display an error message for object types when a limit is reached, but it doesn't specify how many limits are available.</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Could you summarize the information stored about the table of limits in GEO?</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>I don't see any information about "table of limits" in the provided documentation. The available information mentions tables in general, but not specifically "table of limits". If you could provide more context or clarify what you mean by "table of limits", I'll do my best to help.</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>List all the types of limits in the table about GEO limits?</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>According to Table 1 from Data/Introduction\GEO_Limits.htm, the two types of limits are:
+* Types
+* Limits</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>What are the names of each row in the GEO Limits table?</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>The GEO Limits table contains the following fields:
+1. Heading for the field
+2. Size of field in characters
+3. Justification (L/R/C) for Left, Right or Center
+4. Default symbol
+5. Offset of the symbol in Screen units (mm or inches) from the left edge of the track
+6. Specifies zero relative column number to use as deviation/dip in degrees to rotate symbol</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data Demo -1 09 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3567,6 +3567,40 @@
         </is>
       </c>
     </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>What are the size of curve units?</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>The size of curve units is 24.</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>How many queries can be defined per zone type?</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>According to the document, there are 75 query definitions per zone type.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Input Processing -1 10 03 25
✔ Clears the input field after the user has sent their message.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3601,6 +3601,40 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>What is the upper limit on lithology types in a log?</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>The upper limit on lithology types in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>How many lithology types can a single log accommodate at maximum?</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Standardize Processing Question Display -1 10 03 25
✅ Made display of "Processing your question..." function reusable across all functions.
✅ Ensures identical formatting everywhere with a new function "formatAnswerContainer()"
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3635,6 +3635,244 @@
         </is>
       </c>
     </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any one time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>What is the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>What's the maximum number of lithology types in an log?</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>The highest number of lithology types that can be represented in a log is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>How many tracks can you define in one ODF?</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>The maximum number of tracks that can be specified within a single ODF file is 200 tracks at most.</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>How many curve shades can I create?</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>You can create up to 250 curve shades in one ODF.</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>How many curves can I load in one go?</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>According to the document, you can load 450 curves in one go.</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>What the maximum number of headers I can display in my log?</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>How many tables can I have in my log?</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>You can have up to 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Whats the maximum number of characters in a single text entry?</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>32000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>How many symbols can I have in the plot at any one time?</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>You can have up to 10,000 symbols in a plot at any one time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>How many scales can I define?</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>According to the document, you can define up to 23 scales.</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>What the maximum number of data files I can load?</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>The maximum number of data files you can load is unlimited.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Store AI-generated chat titles -1 11 03 25
✅ Ensures the frontend UI updates correctly without redundant title generation
✅ Saves chat session id and chat name as the meta data in the "sessions_metadata.json" file after the AI algorithm generates the chat title.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,9 +433,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="86" customWidth="1" min="1" max="1"/>
+    <col width="94" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="733" customWidth="1" min="3" max="3"/>
+    <col width="785" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3873,6 +3873,68 @@
         </is>
       </c>
     </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>You cannot add 251 curve shades to your log because the maximum number of curve shades per plot is 250.</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>To apply a curve shading with the specified name, follow these steps:
+1. On the Curve tab, select Curve Shading.
+2. The Curve Shading Information dialog box will open.
+3. From Curve Shading, select an unused curve number.
+4. Select Display Curve Shadeto display the shading on the plot.
+5. Enter a curve shadingName as "Hydrocarbon bearing zone highlighted".
+6. Select the Track where the GR curve displays.
+7. In To select &lt;fixed curve value&gt;, enter 40.
+8. In the Zone Attributes grid, Type column, select Pattern.
+9. In the Pattern column, select Sandstone.
+10. Note: Sandstone.vob must be present in your ODF file as a lithology.
+This will apply the specified curve shading with the name "Hydrocarbon bearing zone highlighted" to the GR curve when its value is less than 40 API.</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because the system has a limit on the number of modifiers that can be applied to a single well log. This is specified in the GEO application's documentation under "Modifiers" section, which states that there are 20000 allowed modifiers per plot.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Button Standardization -1 11 03 25
I formatted the responses following the latest chat updates.
Added more standardized CSS sheets for formatting the display of the updated buttons.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3935,6 +3935,40 @@
         </is>
       </c>
     </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>How many log headers can I add to my log?</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>The maximum number of headers you can display in your log is up to 50.</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>You are allowed to create up to 64 tadpole definitions.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Onclick fixing -1 11 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3969,6 +3969,40 @@
         </is>
       </c>
     </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>You are allowed to create up to 64 tadpole definitions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions can I make?</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>You can create up to 64 tadpole definitions.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Comments Improvement -1 11 03 25
✔ Clickable Toggle Icon (🔽 / 🔼)

Clicking this expands/collapses the feedback comment section.
✔ Clickable Star Ratings
Users can set a rating by clicking a star.
✔ Feedback Submission Button
Users can submit ratings and comments by clicking the ➢ button.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4003,6 +4003,23 @@
         </is>
       </c>
     </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions can I make?</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>You are allowed to create up to 64 tadpole definitions.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔧Improve Feedback Handling in RAG Model
12 03 25 Update -1.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <cols>
     <col width="94" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="785" customWidth="1" min="3" max="3"/>
+    <col width="1089" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4020,6 +4020,279 @@
         </is>
       </c>
     </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>You cannot add 251 curve shades to your log because the maximum number of curve shades per plot is 250.</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Unfortunately, I was unable to find any information on the maximum number of data points allowed per curve in the provided documentation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Unfortunately, I was unable to find any information on the maximum number of data points allowed per curve in the provided documentation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>According to the Document section, the answer is:
+You can load an unlimited number of data files.</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Unfortunately, I was unable to find any information on the maximum number of data points allowed per curve in the provided documentation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>The maximum number of data points allowed per curve is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Click "OK" to apply the changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Click "OK" to apply the changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Click "OK" to apply the changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" tab in the GEO application and select "Shading" from the dropdown menu. Then, enter "Hydrocarbon bearing zone highlighted" in the "Shading Name" field and press Enter.</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" tab in the GEO application and select "Shading" from the dropdown menu. Then, enter "Hydrocarbon bearing zone highlighted" in the "Shading Name" field and press Enter.</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Click "OK" to apply the changes.
+Note: The character length of the curve shade name should be within the allowed limit to avoid any errors or issues with the application.</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Click "OK" to apply the changes.
+Note: The character length of the curve shade name should be within the allowed limit to avoid any errors or issues with the application.</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Based on the provided feedback, here's an optimized answer:
+**I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"**
+To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Note that the character limit for the curve shade name is 20 characters; ensure your chosen name does not exceed this limit to avoid any errors or issues with the application.
+This answer addresses the feedback by:
+1. Providing a clear step-by-step guide on how to set the curve shading name.
+2. Mentioning the character limit of 20 characters for the curve shade name, which was previously mentioned in one of the feedback responses.
+3. Encouraging the user to check if their chosen name exceeds the character limit and make a decision accordingly.
+This optimized answer should provide a more accurate and helpful response to the user's question while also addressing the concerns raised in the feedback.</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Here is an optimized answer:
+I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted".
+To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field.
+Note that the character limit for the curve shade name is 20 characters. Since your chosen name has a length of 37 characters, it exceeds the allowed limit. Therefore, this operation is not allowed due to the character length constraint.
+This answer addresses the feedback by:
+1. Providing a clear step-by-step guide on how to set the curve shading name.
+2. Mentioning the character limit of 20 characters for the curve shade name and explaining why the operation is not allowed due to exceeding this limit.
+3. Encouraging the user to check if their chosen name exceeds the character limit and make a decision accordingly.
+This optimized answer should provide a more accurate and helpful response to the user's question while also addressing the concerns raised in the feedback.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tailored Feedback Filtering -1 12 03 25
Included tailored feedback to ensure that the feedback improves only relevant questions that it is related with.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4293,6 +4293,88 @@
         </is>
       </c>
     </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Here is an optimized answer:
+I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted".
+To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field.
+Note that the character limit for the curve shade name is 20 characters. Since your chosen name has a length of 37 characters, it exceeds the allowed limit. Therefore, this operation is not allowed due to the character length constraint.
+This answer addresses the feedback by:
+1. Providing a clear step-by-step guide on how to set the curve shading name.
+2. Mentioning the character limit of 20 characters for the curve shade name and explaining why the operation is not allowed due to exceeding this limit.
+3. Encouraging the user to check if their chosen name exceeds the character limit and make a decision accordingly.
+This optimized answer should provide a more accurate and helpful response to the user's question while also addressing the concerns raised in the feedback.</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Here is an optimized answer:
+"I want to add this name as my curve shade name length \"Hydrocarbon bearing zone highlighted\".
+To set the curve shading name, click on the \"Curve\" menu and select \"Shading\". Then, in the \"Shading\" dialog box, enter \"Hydrocarbon bearing zone highlighted\" in the \"Name\" field.
+Note that the character limit for the curve shade name is 20 characters. Since your chosen name has a length of 37 characters, it exceeds the allowed limit. Therefore, this operation is not allowed due to the character length constraint."</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Here is an optimized answer:
+"I want to add this name as my curve shade name length \"Hydrocarbon bearing zone highlighted\".
+To set the curve shading name, click on the \"Curve\" menu and select \"Shading\". Then, in the \"Shading\" dialog box, enter \"Hydrocarbon bearing zone highlighted\" in the \"Name\" field.
+Note that the character limit for the curve shade name is 20 characters. Since your chosen name has a length of 37 characters, it exceeds the allowed limit. Therefore, this operation is not allowed due to the character length constraint."</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Loaded Relevant Comments -1 12 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4375,6 +4375,210 @@
         </is>
       </c>
     </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>According to the document, you are allowed to create a maximum of 50 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>You are allowed to create a maximum of 5 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Reinforcement Learning -1 12 03 25
Applied Reinforcement Learning to improve the model's response quality on set 2 of Q & As.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C236"/>
+  <dimension ref="A1:C242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4579,6 +4579,111 @@
         </is>
       </c>
     </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>According to Document 30, the maximum number of data files you can load is unlimited. However, it does not specify the maximum number of curves per data file.
+To answer your question accurately, let's look at another document that might provide more information on this topic.
+Document 29 states: "Deviation from the above may cause errors during loading data from files." It also mentions that if possible, you should ask for LAS files from your data provider. However, it does not specify a maximum number of curves per file.
+Unfortunately, without further information or clarification, I cannot provide an accurate answer to your question about the maximum number of curves you can load in a single data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Why can I not add another layout to my log?</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>According to the document, if adding a layout to an existing 'blank' session of GEO, you should load an existing Vew file or create a new one. If adding a layout to an odf with layouts already defined, you need to create the layout first (step 1-2), which will create a copy of the layout currently opened, and then you can overwrite its contents by loading a view file or creating a new one by editing the existing tracks.</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Why can I not add another layout to my log?</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>According to the document, if adding a layout to an existing 'blank' session of GEO, you should load an existing Vew file or create a new one. If adding a layout to an odf with layouts already defined, you need to create the layout first (step 1-2), which will create a copy of the layout currently opened, and then you can overwrite its contents by loading a view file or creating a new one by editing the existing tracks.</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Why can I not add another layout to my log?</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>According to the document, you cannot add another layout to your log because the layout specifies up to 19 layouts per ODF file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>According to document 25, the maximum number of curve shades per plot is 250. This means you cannot add more than 250 curve shades to your log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit specified on theHometab.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Set 2 Question Responses -1 13 03 25
I completed the training on the second set of questions for the models.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C242"/>
+  <dimension ref="A1:C254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4684,6 +4684,220 @@
         </is>
       </c>
     </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>According to Document 30, the maximum number of data files you can load is unlimited. However, it does not specify the maximum number of curves per data file.
+To answer your question accurately, let's look at another document that might provide more information on this topic.
+Document 29 states: "Deviation from the above may cause errors during loading data from files." It also mentions that if possible, you should ask for LAS files from your data provider. However, it does not specify a maximum number of curves per file.
+Another relevant document is Document 27, which states: "Curve shade name length" with a value of 20. This might imply that the maximum curve name length is 20 characters, but it doesn't provide information on the maximum number of curves you can load in a single data file.
+Based on these documents, I couldn't find any specific information on the maximum number of curves you can load in a data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>What is the limit to the number of columns per data file?</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Based on Document 31, which states: "Columns per data file", the maximum number of columns that can be loaded in a GEO file value is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Can curves be loaded into columns?</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Yes, curves can be loaded into columns in GEO. To do this, select the table containing the data you want to display as a curve, then click "Select Curves..." and enter a Curve Mnemonic for each Table Column you wish to generate a curve from. The maximum number of columns that can be loaded is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>What's the maximum number of curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>What's the maximum number of curves I can load?</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is: You can load up to 200 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>What's the maximum number of curves I can load?</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is: You can load up to 450 tracks (curves) per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Question 10: What's the maximum number of curves I can load?</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is: You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Set 2 Questions completed -1 14 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4898,6 +4898,145 @@
         </is>
       </c>
     </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Note that the character limit for the curve shade name is 20 characters; ensure your chosen name does not exceed this limit to avoid any errors or issues with the application.</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load an unlimited number of data points per curve.</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>According to Document 25, the maximum number of curve shades per plot is 250. This means you cannot add more than 250 curve shades to your log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit specified on theHometab.</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>How many log headers can I add to my log?</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Based on the provided feedback, it seems that the correct answer is not explicitly stated in the documentation. However, it does mention that you can select up to 50 headers for display in a log. Therefore, the optimized answer would be:
+"The maximum number of headers you can add to your log is 50."</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>How many tadpole definitions am I allowed?</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>You are allowed to create a maximum of 5 new tadpole definition templates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Why can I not add another layout to my log?</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>According to the document, you cannot add another layout to your log because the layout specifies up to 19 layouts per ODF file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Timed Response Store Demo -1 17 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C262"/>
+  <dimension ref="A1:C266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="94" customWidth="1" min="1" max="1"/>
+    <col width="96" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="1089" customWidth="1" min="3" max="3"/>
   </cols>
@@ -5037,6 +5037,75 @@
         </is>
       </c>
     </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length \"Hydrocarbon bearing zone highlighted\"</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>To set the curve shading name, click on the "Curve" menu and select "Shading". Then, in the "Shading" dialog box, enter "Hydrocarbon bearing zone highlighted" in the "Name" field. Note that the character limit for the curve shade name is 20 characters. Since your chosen name has a length of 37 characters, it exceeds the allowed limit. Therefore, this operation is not allowed due to the character length constraint.</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>According to Document 25, the maximum number of curve shades per plot is 250. This means you cannot add more than 250 curve shades to your log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit specified on theHometab.</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>What's the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load an unlimited number of data points per curve.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed redundant print statements -1 17 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C266"/>
+  <dimension ref="A1:C267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5106,6 +5106,24 @@
         </is>
       </c>
     </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Based on Document 29, which states: "Deviation from the above may cause errors during loading data from files." and considering that the curves are being loaded into columns in Geo so the maximum number of curves correspond to the maximum number of columns in the data file, the answer is:
+You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prompt Engineering -1 17 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C267"/>
+  <dimension ref="A1:C273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5124,6 +5124,108 @@
         </is>
       </c>
     </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>What's the maximum curves I can load in a data file?</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 19.</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because you reached the limit for the number of layouts per ODF file, which is 19.</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prompt Engineering -2 17 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C278"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5226,6 +5226,91 @@
         </is>
       </c>
     </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Model Optimisation -1 17 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C278"/>
+  <dimension ref="A1:C281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5311,6 +5311,57 @@
         </is>
       </c>
     </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 100 tables in a log.</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 20000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Why can I not add another layout to my log?</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>You cannot add another layout to your log because you have reached the limit of 19 layouts per ODF file, as specified by the GEO application.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Run function Time Analysis -1 18 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C287"/>
+  <dimension ref="A1:C288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5464,6 +5464,23 @@
         </is>
       </c>
     </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>The operation is not allowed due to the character length constraint, as the chosen name "Hydrocarbon bearing zone highlighted" has a length of 37 characters, exceeding the allowed limit of 20 characters.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Run function Time Analysis -2 18 03 25
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C288"/>
+  <dimension ref="A1:C292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5481,6 +5481,74 @@
         </is>
       </c>
     </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>You cannot add 251 curve shades to your log because the limit is 250.</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 20000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 20000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>How many log headers can I add to my log?</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Based on the provided feedback, you can select up to 50 headers for display in your log.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Solved offline issue 21 03 25
Ensured that the app could generate a response in an offline environment.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C292"/>
+  <dimension ref="A1:C293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5549,6 +5549,23 @@
         </is>
       </c>
     </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>You cannot add 251 curve shades to your log because the limit is 250.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Q DEMO -1 24 03 25
Conducted a successful test on the model after refactoring the code.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C293"/>
+  <dimension ref="A1:C294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5566,6 +5566,23 @@
         </is>
       </c>
     </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>The operation is not allowed due to the character length constraint, as the chosen name "Hydrocarbon bearing zone highlighted" has a length of 37 characters, exceeding the allowed limit of 20 characters.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Semantic Search UI Design -1 24 04 25
Introduced a new page "semantic_search_page" for conducting semantic searches.
Integrate the changes by updating the menu.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C317"/>
+  <dimension ref="A1:C318"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5976,6 +5976,23 @@
         </is>
       </c>
     </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>I want to add this name as my curve shade name length "Hydrocarbon bearing zone highlighted"</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>The operation is not allowed due to the character length constraint, as the chosen name "Hydrocarbon bearing zone highlighted" has a length of 37 characters, exceeding the allowed limit of 20 characters.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Knowledge Tree Visualization -1
I successfully visualized a knowledge tree showing the relationships between transcript elements loaded from a YouTube Video.
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C318"/>
+  <dimension ref="A1:C319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5993,6 +5993,23 @@
         </is>
       </c>
     </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>I have 20000 modifiers added ty log, why I can't I add anymore?</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>You cannot add more than 20000 modifiers per plot because of the limit on the number of layouts per ODF file. The maximum number of layouts allowed is 20000.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ODF Template Demo 1 (29 04 25).
</commit_message>
<xml_diff>
--- a/Data/query_responses.xlsx
+++ b/Data/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C319"/>
+  <dimension ref="A1:C323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6010,6 +6010,82 @@
         </is>
       </c>
     </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>How many types of information can an ODT file hold?</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>According to the provided documents, an ODT file can hold encapsulated geological information such as Gas data, descriptions, lithology, % lithology, table/curve parameter details and qualitative information.</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Which type of content can be viewed from an ODT file?</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>According to the Documents section, an ODT file contains:
+1. Library information (headers, lithology, modifiers, structures, and symbols)
+2. View file contents (track layout information, depth and screen units, scale and pen information)
+3. ini file settings (curve defaults, computed curves and table definitions)
+Therefore, an ODT file can be viewed as containing all of these types of content.</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>List the library informations from an ODT file</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Based on the provided documents, to list library information from an ODT file, you can:
+1. Open the template by selecting "Templat" on the GEOMenu.
+2. In the Open Template dialog box, browse to the location of your ODT file and select it.
+3. Click "Open".
+The document information tree will be displayed, showing warnings if some components are not functioning correctly or have settings that are deemed not best practice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Can an ODT be created from an existing ODF file?</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Yes, an ODT (OpenDocument Template) can be created from an existing ODF (OpenDocument Format) file by selecting "Save as" and then choosing the template option. Alternatively, you can also create a new ODT directly from an ODF using the "Create Template" function in the GEO menu.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>